<commit_message>
fixed raycaster bug and updated spready
</commit_message>
<xml_diff>
--- a/Ressources/Documentation/RPG Stats Spreadsheet.xlsx
+++ b/Ressources/Documentation/RPG Stats Spreadsheet.xlsx
@@ -1,14 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Player" sheetId="1" r:id="rId1"/>
-    <sheet name="Enemies" sheetId="2" r:id="rId2"/>
+    <sheet name="Soul" sheetId="3" r:id="rId1"/>
+    <sheet name="Player" sheetId="4" r:id="rId2"/>
+    <sheet name="Old - Player" sheetId="1" r:id="rId3"/>
+    <sheet name="Old - Enemies" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
   <si>
     <t>Player Level</t>
   </si>
@@ -74,13 +76,97 @@
   </si>
   <si>
     <t>Chase Radius</t>
+  </si>
+  <si>
+    <t>Aspect</t>
+  </si>
+  <si>
+    <t>Element</t>
+  </si>
+  <si>
+    <t>Approach</t>
+  </si>
+  <si>
+    <t>Hits to kill</t>
+  </si>
+  <si>
+    <t>Abilities</t>
+  </si>
+  <si>
+    <t>Hits to kill enemy at same level</t>
+  </si>
+  <si>
+    <t>Hits to kill player at same level</t>
+  </si>
+  <si>
+    <t>Increase of damage</t>
+  </si>
+  <si>
+    <t># of abilities casts for full energy</t>
+  </si>
+  <si>
+    <t>speed to reach full energy</t>
+  </si>
+  <si>
+    <t>x3</t>
+  </si>
+  <si>
+    <t>x1.5</t>
+  </si>
+  <si>
+    <t>20 secs</t>
+  </si>
+  <si>
+    <t>Player Details</t>
+  </si>
+  <si>
+    <t>XP to level up</t>
+  </si>
+  <si>
+    <t>Typical Ability Damage</t>
+  </si>
+  <si>
+    <t>Base enemy details</t>
+  </si>
+  <si>
+    <t>Big Hit Damage</t>
+  </si>
+  <si>
+    <t>Multiplier</t>
+  </si>
+  <si>
+    <t>XP per enemy kill</t>
+  </si>
+  <si>
+    <t>Leveling up</t>
+  </si>
+  <si>
+    <t>Enemy kills to level up at lvl 1</t>
+  </si>
+  <si>
+    <t>XP per enemy at lvl 1</t>
+  </si>
+  <si>
+    <t>% increase in number of kills to level up</t>
+  </si>
+  <si>
+    <t>% xp increase for level up</t>
+  </si>
+  <si>
+    <t>XP to level up at lvl 1</t>
+  </si>
+  <si>
+    <t>XP per enemy at lvl 2</t>
+  </si>
+  <si>
+    <t>enemy kills to lvl up</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,8 +200,17 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,6 +220,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -152,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -173,6 +280,11 @@
     <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -453,10 +565,2321 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="36.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12">
+        <f>(D12-C9)/C9*100</f>
+        <v>40</v>
+      </c>
+      <c r="D12">
+        <v>35</v>
+      </c>
+      <c r="E12">
+        <f>D12-C9</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13">
+        <v>100</v>
+      </c>
+      <c r="D13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14">
+        <v>4000</v>
+      </c>
+      <c r="D14">
+        <v>2000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K103"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="8">
+        <v>3</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="8">
+        <v>2000</v>
+      </c>
+      <c r="C3" s="8">
+        <v>20</v>
+      </c>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8">
+        <v>40</v>
+      </c>
+      <c r="F3" s="8">
+        <v>5</v>
+      </c>
+      <c r="G3" s="8"/>
+      <c r="I3" s="9">
+        <v>2</v>
+      </c>
+      <c r="J3" s="9">
+        <v>20</v>
+      </c>
+      <c r="K3" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="12">
+        <v>2000</v>
+      </c>
+      <c r="C4" s="12">
+        <v>80</v>
+      </c>
+      <c r="D4" s="12">
+        <f>B4/C4</f>
+        <v>25</v>
+      </c>
+      <c r="E4" s="12">
+        <v>200</v>
+      </c>
+      <c r="F4" s="12">
+        <v>10</v>
+      </c>
+      <c r="G4" s="12">
+        <f>F4*$G$1</f>
+        <v>30</v>
+      </c>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12">
+        <f>F4*$I$3</f>
+        <v>20</v>
+      </c>
+      <c r="J4" s="12">
+        <f>E4/$J$3</f>
+        <v>10</v>
+      </c>
+      <c r="K4" s="12">
+        <f>J4*$K$1</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="12">
+        <f>B4+$B$3</f>
+        <v>4000</v>
+      </c>
+      <c r="C5" s="12">
+        <f>C4+$C$3</f>
+        <v>100</v>
+      </c>
+      <c r="D5" s="12">
+        <f t="shared" ref="D5:D23" si="0">B5/C5</f>
+        <v>40</v>
+      </c>
+      <c r="E5" s="12">
+        <f>E4+$E$3</f>
+        <v>240</v>
+      </c>
+      <c r="F5" s="12">
+        <f>F4+$F$3</f>
+        <v>15</v>
+      </c>
+      <c r="G5" s="12">
+        <f t="shared" ref="G5:G23" si="1">F5*$G$1</f>
+        <v>45</v>
+      </c>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12">
+        <f t="shared" ref="I5:I23" si="2">F5*$I$3</f>
+        <v>30</v>
+      </c>
+      <c r="J5" s="12">
+        <f t="shared" ref="J5:J23" si="3">E5/$J$3</f>
+        <v>12</v>
+      </c>
+      <c r="K5" s="12">
+        <f t="shared" ref="K5:K23" si="4">J5*$K$1</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="12">
+        <f t="shared" ref="B6:B23" si="5">B5+$B$3</f>
+        <v>6000</v>
+      </c>
+      <c r="C6" s="12">
+        <f t="shared" ref="C6:C23" si="6">C5+$C$3</f>
+        <v>120</v>
+      </c>
+      <c r="D6" s="12">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="E6" s="12">
+        <f t="shared" ref="E6:E23" si="7">E5+$E$3</f>
+        <v>280</v>
+      </c>
+      <c r="F6" s="12">
+        <f t="shared" ref="F6:F23" si="8">F5+$F$3</f>
+        <v>20</v>
+      </c>
+      <c r="G6" s="12">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="J6" s="12">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="K6" s="12">
+        <f t="shared" si="4"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="12">
+        <f t="shared" si="5"/>
+        <v>8000</v>
+      </c>
+      <c r="C7" s="12">
+        <f t="shared" si="6"/>
+        <v>140</v>
+      </c>
+      <c r="D7" s="12">
+        <f t="shared" si="0"/>
+        <v>57.142857142857146</v>
+      </c>
+      <c r="E7" s="12">
+        <f t="shared" si="7"/>
+        <v>320</v>
+      </c>
+      <c r="F7" s="12">
+        <f t="shared" si="8"/>
+        <v>25</v>
+      </c>
+      <c r="G7" s="12">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="J7" s="12">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="K7" s="12">
+        <f t="shared" si="4"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" s="12">
+        <f t="shared" si="5"/>
+        <v>10000</v>
+      </c>
+      <c r="C8" s="12">
+        <f t="shared" si="6"/>
+        <v>160</v>
+      </c>
+      <c r="D8" s="12">
+        <f t="shared" si="0"/>
+        <v>62.5</v>
+      </c>
+      <c r="E8" s="12">
+        <f t="shared" si="7"/>
+        <v>360</v>
+      </c>
+      <c r="F8" s="12">
+        <f t="shared" si="8"/>
+        <v>30</v>
+      </c>
+      <c r="G8" s="12">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="J8" s="12">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="K8" s="12">
+        <f t="shared" si="4"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="12">
+        <f t="shared" si="5"/>
+        <v>12000</v>
+      </c>
+      <c r="C9" s="12">
+        <f t="shared" si="6"/>
+        <v>180</v>
+      </c>
+      <c r="D9" s="12">
+        <f t="shared" si="0"/>
+        <v>66.666666666666671</v>
+      </c>
+      <c r="E9" s="12">
+        <f t="shared" si="7"/>
+        <v>400</v>
+      </c>
+      <c r="F9" s="12">
+        <f t="shared" si="8"/>
+        <v>35</v>
+      </c>
+      <c r="G9" s="12">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="J9" s="12">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="K9" s="12">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" s="12">
+        <f t="shared" si="5"/>
+        <v>14000</v>
+      </c>
+      <c r="C10" s="12">
+        <f t="shared" si="6"/>
+        <v>200</v>
+      </c>
+      <c r="D10" s="12">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="E10" s="12">
+        <f t="shared" si="7"/>
+        <v>440</v>
+      </c>
+      <c r="F10" s="12">
+        <f t="shared" si="8"/>
+        <v>40</v>
+      </c>
+      <c r="G10" s="12">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="J10" s="12">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="K10" s="12">
+        <f t="shared" si="4"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" s="12">
+        <f t="shared" si="5"/>
+        <v>16000</v>
+      </c>
+      <c r="C11" s="12">
+        <f t="shared" si="6"/>
+        <v>220</v>
+      </c>
+      <c r="D11" s="12">
+        <f t="shared" si="0"/>
+        <v>72.727272727272734</v>
+      </c>
+      <c r="E11" s="12">
+        <f t="shared" si="7"/>
+        <v>480</v>
+      </c>
+      <c r="F11" s="12">
+        <f t="shared" si="8"/>
+        <v>45</v>
+      </c>
+      <c r="G11" s="12">
+        <f t="shared" si="1"/>
+        <v>135</v>
+      </c>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="J11" s="12">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="K11" s="12">
+        <f t="shared" si="4"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" s="12">
+        <f t="shared" si="5"/>
+        <v>18000</v>
+      </c>
+      <c r="C12" s="12">
+        <f t="shared" si="6"/>
+        <v>240</v>
+      </c>
+      <c r="D12" s="12">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="E12" s="12">
+        <f t="shared" si="7"/>
+        <v>520</v>
+      </c>
+      <c r="F12" s="12">
+        <f t="shared" si="8"/>
+        <v>50</v>
+      </c>
+      <c r="G12" s="12">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="J12" s="12">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="K12" s="12">
+        <f t="shared" si="4"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" s="12">
+        <f t="shared" si="5"/>
+        <v>20000</v>
+      </c>
+      <c r="C13" s="12">
+        <f t="shared" si="6"/>
+        <v>260</v>
+      </c>
+      <c r="D13" s="12">
+        <f t="shared" si="0"/>
+        <v>76.92307692307692</v>
+      </c>
+      <c r="E13" s="12">
+        <f t="shared" si="7"/>
+        <v>560</v>
+      </c>
+      <c r="F13" s="12">
+        <f t="shared" si="8"/>
+        <v>55</v>
+      </c>
+      <c r="G13" s="12">
+        <f t="shared" si="1"/>
+        <v>165</v>
+      </c>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12">
+        <f t="shared" si="2"/>
+        <v>110</v>
+      </c>
+      <c r="J13" s="12">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="K13" s="12">
+        <f t="shared" si="4"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" s="12">
+        <f t="shared" si="5"/>
+        <v>22000</v>
+      </c>
+      <c r="C14" s="12">
+        <f t="shared" si="6"/>
+        <v>280</v>
+      </c>
+      <c r="D14" s="12">
+        <f t="shared" si="0"/>
+        <v>78.571428571428569</v>
+      </c>
+      <c r="E14" s="12">
+        <f t="shared" si="7"/>
+        <v>600</v>
+      </c>
+      <c r="F14" s="12">
+        <f t="shared" si="8"/>
+        <v>60</v>
+      </c>
+      <c r="G14" s="12">
+        <f t="shared" si="1"/>
+        <v>180</v>
+      </c>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
+      <c r="J14" s="12">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="K14" s="12">
+        <f t="shared" si="4"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" s="12">
+        <f t="shared" si="5"/>
+        <v>24000</v>
+      </c>
+      <c r="C15" s="12">
+        <f t="shared" si="6"/>
+        <v>300</v>
+      </c>
+      <c r="D15" s="12">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="E15" s="12">
+        <f t="shared" si="7"/>
+        <v>640</v>
+      </c>
+      <c r="F15" s="12">
+        <f t="shared" si="8"/>
+        <v>65</v>
+      </c>
+      <c r="G15" s="12">
+        <f t="shared" si="1"/>
+        <v>195</v>
+      </c>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12">
+        <f t="shared" si="2"/>
+        <v>130</v>
+      </c>
+      <c r="J15" s="12">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="K15" s="12">
+        <f t="shared" si="4"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" s="12">
+        <f t="shared" si="5"/>
+        <v>26000</v>
+      </c>
+      <c r="C16" s="12">
+        <f t="shared" si="6"/>
+        <v>320</v>
+      </c>
+      <c r="D16" s="12">
+        <f t="shared" si="0"/>
+        <v>81.25</v>
+      </c>
+      <c r="E16" s="12">
+        <f t="shared" si="7"/>
+        <v>680</v>
+      </c>
+      <c r="F16" s="12">
+        <f t="shared" si="8"/>
+        <v>70</v>
+      </c>
+      <c r="G16" s="12">
+        <f t="shared" si="1"/>
+        <v>210</v>
+      </c>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12">
+        <f t="shared" si="2"/>
+        <v>140</v>
+      </c>
+      <c r="J16" s="12">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+      <c r="K16" s="12">
+        <f t="shared" si="4"/>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17" s="12">
+        <f t="shared" si="5"/>
+        <v>28000</v>
+      </c>
+      <c r="C17" s="12">
+        <f t="shared" si="6"/>
+        <v>340</v>
+      </c>
+      <c r="D17" s="12">
+        <f t="shared" si="0"/>
+        <v>82.352941176470594</v>
+      </c>
+      <c r="E17" s="12">
+        <f t="shared" si="7"/>
+        <v>720</v>
+      </c>
+      <c r="F17" s="12">
+        <f t="shared" si="8"/>
+        <v>75</v>
+      </c>
+      <c r="G17" s="12">
+        <f t="shared" si="1"/>
+        <v>225</v>
+      </c>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
+      <c r="J17" s="12">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="K17" s="12">
+        <f t="shared" si="4"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18" s="12">
+        <f t="shared" si="5"/>
+        <v>30000</v>
+      </c>
+      <c r="C18" s="12">
+        <f t="shared" si="6"/>
+        <v>360</v>
+      </c>
+      <c r="D18" s="12">
+        <f t="shared" si="0"/>
+        <v>83.333333333333329</v>
+      </c>
+      <c r="E18" s="12">
+        <f t="shared" si="7"/>
+        <v>760</v>
+      </c>
+      <c r="F18" s="12">
+        <f t="shared" si="8"/>
+        <v>80</v>
+      </c>
+      <c r="G18" s="12">
+        <f t="shared" si="1"/>
+        <v>240</v>
+      </c>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12">
+        <f t="shared" si="2"/>
+        <v>160</v>
+      </c>
+      <c r="J18" s="12">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="K18" s="12">
+        <f t="shared" si="4"/>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19" s="12">
+        <f t="shared" si="5"/>
+        <v>32000</v>
+      </c>
+      <c r="C19" s="12">
+        <f t="shared" si="6"/>
+        <v>380</v>
+      </c>
+      <c r="D19" s="12">
+        <f t="shared" si="0"/>
+        <v>84.21052631578948</v>
+      </c>
+      <c r="E19" s="12">
+        <f t="shared" si="7"/>
+        <v>800</v>
+      </c>
+      <c r="F19" s="12">
+        <f t="shared" si="8"/>
+        <v>85</v>
+      </c>
+      <c r="G19" s="12">
+        <f t="shared" si="1"/>
+        <v>255</v>
+      </c>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12">
+        <f t="shared" si="2"/>
+        <v>170</v>
+      </c>
+      <c r="J19" s="12">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="K19" s="12">
+        <f t="shared" si="4"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20" s="12">
+        <f t="shared" si="5"/>
+        <v>34000</v>
+      </c>
+      <c r="C20" s="12">
+        <f t="shared" si="6"/>
+        <v>400</v>
+      </c>
+      <c r="D20" s="12">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+      <c r="E20" s="12">
+        <f t="shared" si="7"/>
+        <v>840</v>
+      </c>
+      <c r="F20" s="12">
+        <f t="shared" si="8"/>
+        <v>90</v>
+      </c>
+      <c r="G20" s="12">
+        <f t="shared" si="1"/>
+        <v>270</v>
+      </c>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12">
+        <f t="shared" si="2"/>
+        <v>180</v>
+      </c>
+      <c r="J20" s="12">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="K20" s="12">
+        <f t="shared" si="4"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21" s="12">
+        <f t="shared" si="5"/>
+        <v>36000</v>
+      </c>
+      <c r="C21" s="12">
+        <f t="shared" si="6"/>
+        <v>420</v>
+      </c>
+      <c r="D21" s="12">
+        <f t="shared" si="0"/>
+        <v>85.714285714285708</v>
+      </c>
+      <c r="E21" s="12">
+        <f t="shared" si="7"/>
+        <v>880</v>
+      </c>
+      <c r="F21" s="12">
+        <f t="shared" si="8"/>
+        <v>95</v>
+      </c>
+      <c r="G21" s="12">
+        <f t="shared" si="1"/>
+        <v>285</v>
+      </c>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12">
+        <f t="shared" si="2"/>
+        <v>190</v>
+      </c>
+      <c r="J21" s="12">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="K21" s="12">
+        <f t="shared" si="4"/>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22" s="12">
+        <f t="shared" si="5"/>
+        <v>38000</v>
+      </c>
+      <c r="C22" s="12">
+        <f t="shared" si="6"/>
+        <v>440</v>
+      </c>
+      <c r="D22" s="12">
+        <f t="shared" si="0"/>
+        <v>86.36363636363636</v>
+      </c>
+      <c r="E22" s="12">
+        <f t="shared" si="7"/>
+        <v>920</v>
+      </c>
+      <c r="F22" s="12">
+        <f t="shared" si="8"/>
+        <v>100</v>
+      </c>
+      <c r="G22" s="12">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12">
+        <f t="shared" si="2"/>
+        <v>200</v>
+      </c>
+      <c r="J22" s="12">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="K22" s="12">
+        <f t="shared" si="4"/>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="B23" s="12">
+        <f t="shared" si="5"/>
+        <v>40000</v>
+      </c>
+      <c r="C23" s="12">
+        <f t="shared" si="6"/>
+        <v>460</v>
+      </c>
+      <c r="D23" s="12">
+        <f t="shared" si="0"/>
+        <v>86.956521739130437</v>
+      </c>
+      <c r="E23" s="12">
+        <f t="shared" si="7"/>
+        <v>960</v>
+      </c>
+      <c r="F23" s="12">
+        <f t="shared" si="8"/>
+        <v>105</v>
+      </c>
+      <c r="G23" s="12">
+        <f t="shared" si="1"/>
+        <v>315</v>
+      </c>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12">
+        <f t="shared" si="2"/>
+        <v>210</v>
+      </c>
+      <c r="J23" s="12">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="K23" s="12">
+        <f t="shared" si="4"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>24</v>
+      </c>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>25</v>
+      </c>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>26</v>
+      </c>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>27</v>
+      </c>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>28</v>
+      </c>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>29</v>
+      </c>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>30</v>
+      </c>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>31</v>
+      </c>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>32</v>
+      </c>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>33</v>
+      </c>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="12"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>34</v>
+      </c>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
+      <c r="K37" s="12"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>35</v>
+      </c>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="12"/>
+      <c r="K38" s="12"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>36</v>
+      </c>
+      <c r="B39" s="12"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="12"/>
+      <c r="J39" s="12"/>
+      <c r="K39" s="12"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>37</v>
+      </c>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="12"/>
+      <c r="K40" s="12"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>38</v>
+      </c>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="12"/>
+      <c r="K41" s="12"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>39</v>
+      </c>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="12"/>
+      <c r="J42" s="12"/>
+      <c r="K42" s="12"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>40</v>
+      </c>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="12"/>
+      <c r="I43" s="12"/>
+      <c r="J43" s="12"/>
+      <c r="K43" s="12"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>41</v>
+      </c>
+      <c r="B44" s="12"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="12"/>
+      <c r="J44" s="12"/>
+      <c r="K44" s="12"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>42</v>
+      </c>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="12"/>
+      <c r="J45" s="12"/>
+      <c r="K45" s="12"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>43</v>
+      </c>
+      <c r="B46" s="12"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="12"/>
+      <c r="J46" s="12"/>
+      <c r="K46" s="12"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>44</v>
+      </c>
+      <c r="B47" s="12"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="12"/>
+      <c r="I47" s="12"/>
+      <c r="J47" s="12"/>
+      <c r="K47" s="12"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>45</v>
+      </c>
+      <c r="B48" s="12"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="12"/>
+      <c r="I48" s="12"/>
+      <c r="J48" s="12"/>
+      <c r="K48" s="12"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>46</v>
+      </c>
+      <c r="B49" s="12"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+      <c r="H49" s="12"/>
+      <c r="I49" s="12"/>
+      <c r="J49" s="12"/>
+      <c r="K49" s="12"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>47</v>
+      </c>
+      <c r="B50" s="12"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="12"/>
+      <c r="H50" s="12"/>
+      <c r="I50" s="12"/>
+      <c r="J50" s="12"/>
+      <c r="K50" s="12"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>48</v>
+      </c>
+      <c r="B51" s="12"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="12"/>
+      <c r="H51" s="12"/>
+      <c r="I51" s="12"/>
+      <c r="J51" s="12"/>
+      <c r="K51" s="12"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>49</v>
+      </c>
+      <c r="B52" s="12"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="12"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="12"/>
+      <c r="H52" s="12"/>
+      <c r="I52" s="12"/>
+      <c r="J52" s="12"/>
+      <c r="K52" s="12"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>50</v>
+      </c>
+      <c r="B53" s="12"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="12"/>
+      <c r="G53" s="12"/>
+      <c r="H53" s="12"/>
+      <c r="I53" s="12"/>
+      <c r="J53" s="12"/>
+      <c r="K53" s="12"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>51</v>
+      </c>
+      <c r="B54" s="12"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
+      <c r="H54" s="12"/>
+      <c r="I54" s="12"/>
+      <c r="J54" s="12"/>
+      <c r="K54" s="12"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>52</v>
+      </c>
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+      <c r="G55" s="12"/>
+      <c r="H55" s="12"/>
+      <c r="I55" s="12"/>
+      <c r="J55" s="12"/>
+      <c r="K55" s="12"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>53</v>
+      </c>
+      <c r="B56" s="12"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="12"/>
+      <c r="H56" s="12"/>
+      <c r="I56" s="12"/>
+      <c r="J56" s="12"/>
+      <c r="K56" s="12"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>54</v>
+      </c>
+      <c r="B57" s="12"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="12"/>
+      <c r="F57" s="12"/>
+      <c r="G57" s="12"/>
+      <c r="H57" s="12"/>
+      <c r="I57" s="12"/>
+      <c r="J57" s="12"/>
+      <c r="K57" s="12"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>55</v>
+      </c>
+      <c r="B58" s="12"/>
+      <c r="C58" s="12"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="12"/>
+      <c r="G58" s="12"/>
+      <c r="H58" s="12"/>
+      <c r="I58" s="12"/>
+      <c r="J58" s="12"/>
+      <c r="K58" s="12"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>56</v>
+      </c>
+      <c r="B59" s="12"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12"/>
+      <c r="F59" s="12"/>
+      <c r="G59" s="12"/>
+      <c r="H59" s="12"/>
+      <c r="I59" s="12"/>
+      <c r="J59" s="12"/>
+      <c r="K59" s="12"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>57</v>
+      </c>
+      <c r="B60" s="12"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="12"/>
+      <c r="H60" s="12"/>
+      <c r="I60" s="12"/>
+      <c r="J60" s="12"/>
+      <c r="K60" s="12"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>58</v>
+      </c>
+      <c r="B61" s="12"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
+      <c r="G61" s="12"/>
+      <c r="H61" s="12"/>
+      <c r="I61" s="12"/>
+      <c r="J61" s="12"/>
+      <c r="K61" s="12"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>59</v>
+      </c>
+      <c r="B62" s="12"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="12"/>
+      <c r="E62" s="12"/>
+      <c r="F62" s="12"/>
+      <c r="G62" s="12"/>
+      <c r="H62" s="12"/>
+      <c r="I62" s="12"/>
+      <c r="J62" s="12"/>
+      <c r="K62" s="12"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>60</v>
+      </c>
+      <c r="B63" s="12"/>
+      <c r="C63" s="12"/>
+      <c r="D63" s="12"/>
+      <c r="E63" s="12"/>
+      <c r="F63" s="12"/>
+      <c r="G63" s="12"/>
+      <c r="H63" s="12"/>
+      <c r="I63" s="12"/>
+      <c r="J63" s="12"/>
+      <c r="K63" s="12"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>61</v>
+      </c>
+      <c r="B64" s="12"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="12"/>
+      <c r="F64" s="12"/>
+      <c r="G64" s="12"/>
+      <c r="H64" s="12"/>
+      <c r="I64" s="12"/>
+      <c r="J64" s="12"/>
+      <c r="K64" s="12"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>62</v>
+      </c>
+      <c r="B65" s="12"/>
+      <c r="C65" s="12"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="12"/>
+      <c r="G65" s="12"/>
+      <c r="H65" s="12"/>
+      <c r="I65" s="12"/>
+      <c r="J65" s="12"/>
+      <c r="K65" s="12"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>63</v>
+      </c>
+      <c r="B66" s="12"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="12"/>
+      <c r="E66" s="12"/>
+      <c r="F66" s="12"/>
+      <c r="G66" s="12"/>
+      <c r="H66" s="12"/>
+      <c r="I66" s="12"/>
+      <c r="J66" s="12"/>
+      <c r="K66" s="12"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>64</v>
+      </c>
+      <c r="B67" s="12"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="12"/>
+      <c r="F67" s="12"/>
+      <c r="G67" s="12"/>
+      <c r="H67" s="12"/>
+      <c r="I67" s="12"/>
+      <c r="J67" s="12"/>
+      <c r="K67" s="12"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>65</v>
+      </c>
+      <c r="B68" s="12"/>
+      <c r="C68" s="12"/>
+      <c r="D68" s="12"/>
+      <c r="E68" s="12"/>
+      <c r="F68" s="12"/>
+      <c r="G68" s="12"/>
+      <c r="H68" s="12"/>
+      <c r="I68" s="12"/>
+      <c r="J68" s="12"/>
+      <c r="K68" s="12"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>66</v>
+      </c>
+      <c r="B69" s="12"/>
+      <c r="C69" s="12"/>
+      <c r="D69" s="12"/>
+      <c r="E69" s="12"/>
+      <c r="F69" s="12"/>
+      <c r="G69" s="12"/>
+      <c r="H69" s="12"/>
+      <c r="I69" s="12"/>
+      <c r="J69" s="12"/>
+      <c r="K69" s="12"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>67</v>
+      </c>
+      <c r="B70" s="12"/>
+      <c r="C70" s="12"/>
+      <c r="D70" s="12"/>
+      <c r="E70" s="12"/>
+      <c r="F70" s="12"/>
+      <c r="G70" s="12"/>
+      <c r="H70" s="12"/>
+      <c r="I70" s="12"/>
+      <c r="J70" s="12"/>
+      <c r="K70" s="12"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>68</v>
+      </c>
+      <c r="B71" s="12"/>
+      <c r="C71" s="12"/>
+      <c r="D71" s="12"/>
+      <c r="E71" s="12"/>
+      <c r="F71" s="12"/>
+      <c r="G71" s="12"/>
+      <c r="H71" s="12"/>
+      <c r="I71" s="12"/>
+      <c r="J71" s="12"/>
+      <c r="K71" s="12"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>69</v>
+      </c>
+      <c r="B72" s="12"/>
+      <c r="C72" s="12"/>
+      <c r="D72" s="12"/>
+      <c r="E72" s="12"/>
+      <c r="F72" s="12"/>
+      <c r="G72" s="12"/>
+      <c r="H72" s="12"/>
+      <c r="I72" s="12"/>
+      <c r="J72" s="12"/>
+      <c r="K72" s="12"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>70</v>
+      </c>
+      <c r="B73" s="12"/>
+      <c r="C73" s="12"/>
+      <c r="D73" s="12"/>
+      <c r="E73" s="12"/>
+      <c r="F73" s="12"/>
+      <c r="G73" s="12"/>
+      <c r="H73" s="12"/>
+      <c r="I73" s="12"/>
+      <c r="J73" s="12"/>
+      <c r="K73" s="12"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>71</v>
+      </c>
+      <c r="B74" s="12"/>
+      <c r="C74" s="12"/>
+      <c r="D74" s="12"/>
+      <c r="E74" s="12"/>
+      <c r="F74" s="12"/>
+      <c r="G74" s="12"/>
+      <c r="H74" s="12"/>
+      <c r="I74" s="12"/>
+      <c r="J74" s="12"/>
+      <c r="K74" s="12"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>72</v>
+      </c>
+      <c r="B75" s="12"/>
+      <c r="C75" s="12"/>
+      <c r="D75" s="12"/>
+      <c r="E75" s="12"/>
+      <c r="F75" s="12"/>
+      <c r="G75" s="12"/>
+      <c r="H75" s="12"/>
+      <c r="I75" s="12"/>
+      <c r="J75" s="12"/>
+      <c r="K75" s="12"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>73</v>
+      </c>
+      <c r="B76" s="12"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="12"/>
+      <c r="G76" s="12"/>
+      <c r="H76" s="12"/>
+      <c r="I76" s="12"/>
+      <c r="J76" s="12"/>
+      <c r="K76" s="12"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>74</v>
+      </c>
+      <c r="B77" s="12"/>
+      <c r="C77" s="12"/>
+      <c r="D77" s="12"/>
+      <c r="E77" s="12"/>
+      <c r="F77" s="12"/>
+      <c r="G77" s="12"/>
+      <c r="H77" s="12"/>
+      <c r="I77" s="12"/>
+      <c r="J77" s="12"/>
+      <c r="K77" s="12"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>75</v>
+      </c>
+      <c r="B78" s="12"/>
+      <c r="C78" s="12"/>
+      <c r="D78" s="12"/>
+      <c r="E78" s="12"/>
+      <c r="F78" s="12"/>
+      <c r="G78" s="12"/>
+      <c r="H78" s="12"/>
+      <c r="I78" s="12"/>
+      <c r="J78" s="12"/>
+      <c r="K78" s="12"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>76</v>
+      </c>
+      <c r="B79" s="12"/>
+      <c r="C79" s="12"/>
+      <c r="D79" s="12"/>
+      <c r="E79" s="12"/>
+      <c r="F79" s="12"/>
+      <c r="G79" s="12"/>
+      <c r="H79" s="12"/>
+      <c r="I79" s="12"/>
+      <c r="J79" s="12"/>
+      <c r="K79" s="12"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>77</v>
+      </c>
+      <c r="B80" s="12"/>
+      <c r="C80" s="12"/>
+      <c r="D80" s="12"/>
+      <c r="E80" s="12"/>
+      <c r="F80" s="12"/>
+      <c r="G80" s="12"/>
+      <c r="H80" s="12"/>
+      <c r="I80" s="12"/>
+      <c r="J80" s="12"/>
+      <c r="K80" s="12"/>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>78</v>
+      </c>
+      <c r="B81" s="12"/>
+      <c r="C81" s="12"/>
+      <c r="D81" s="12"/>
+      <c r="E81" s="12"/>
+      <c r="F81" s="12"/>
+      <c r="G81" s="12"/>
+      <c r="H81" s="12"/>
+      <c r="I81" s="12"/>
+      <c r="J81" s="12"/>
+      <c r="K81" s="12"/>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>79</v>
+      </c>
+      <c r="B82" s="12"/>
+      <c r="C82" s="12"/>
+      <c r="D82" s="12"/>
+      <c r="E82" s="12"/>
+      <c r="F82" s="12"/>
+      <c r="G82" s="12"/>
+      <c r="H82" s="12"/>
+      <c r="I82" s="12"/>
+      <c r="J82" s="12"/>
+      <c r="K82" s="12"/>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>80</v>
+      </c>
+      <c r="B83" s="12"/>
+      <c r="C83" s="12"/>
+      <c r="D83" s="12"/>
+      <c r="E83" s="12"/>
+      <c r="F83" s="12"/>
+      <c r="G83" s="12"/>
+      <c r="H83" s="12"/>
+      <c r="I83" s="12"/>
+      <c r="J83" s="12"/>
+      <c r="K83" s="12"/>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>81</v>
+      </c>
+      <c r="B84" s="12"/>
+      <c r="C84" s="12"/>
+      <c r="D84" s="12"/>
+      <c r="E84" s="12"/>
+      <c r="F84" s="12"/>
+      <c r="G84" s="12"/>
+      <c r="H84" s="12"/>
+      <c r="I84" s="12"/>
+      <c r="J84" s="12"/>
+      <c r="K84" s="12"/>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>82</v>
+      </c>
+      <c r="B85" s="12"/>
+      <c r="C85" s="12"/>
+      <c r="D85" s="12"/>
+      <c r="E85" s="12"/>
+      <c r="F85" s="12"/>
+      <c r="G85" s="12"/>
+      <c r="H85" s="12"/>
+      <c r="I85" s="12"/>
+      <c r="J85" s="12"/>
+      <c r="K85" s="12"/>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>83</v>
+      </c>
+      <c r="B86" s="12"/>
+      <c r="C86" s="12"/>
+      <c r="D86" s="12"/>
+      <c r="E86" s="12"/>
+      <c r="F86" s="12"/>
+      <c r="G86" s="12"/>
+      <c r="H86" s="12"/>
+      <c r="I86" s="12"/>
+      <c r="J86" s="12"/>
+      <c r="K86" s="12"/>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>84</v>
+      </c>
+      <c r="B87" s="12"/>
+      <c r="C87" s="12"/>
+      <c r="D87" s="12"/>
+      <c r="E87" s="12"/>
+      <c r="F87" s="12"/>
+      <c r="G87" s="12"/>
+      <c r="H87" s="12"/>
+      <c r="I87" s="12"/>
+      <c r="J87" s="12"/>
+      <c r="K87" s="12"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>85</v>
+      </c>
+      <c r="B88" s="12"/>
+      <c r="C88" s="12"/>
+      <c r="D88" s="12"/>
+      <c r="E88" s="12"/>
+      <c r="F88" s="12"/>
+      <c r="G88" s="12"/>
+      <c r="H88" s="12"/>
+      <c r="I88" s="12"/>
+      <c r="J88" s="12"/>
+      <c r="K88" s="12"/>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>86</v>
+      </c>
+      <c r="B89" s="12"/>
+      <c r="C89" s="12"/>
+      <c r="D89" s="12"/>
+      <c r="E89" s="12"/>
+      <c r="F89" s="12"/>
+      <c r="G89" s="12"/>
+      <c r="H89" s="12"/>
+      <c r="I89" s="12"/>
+      <c r="J89" s="12"/>
+      <c r="K89" s="12"/>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>87</v>
+      </c>
+      <c r="B90" s="12"/>
+      <c r="C90" s="12"/>
+      <c r="D90" s="12"/>
+      <c r="E90" s="12"/>
+      <c r="F90" s="12"/>
+      <c r="G90" s="12"/>
+      <c r="H90" s="12"/>
+      <c r="I90" s="12"/>
+      <c r="J90" s="12"/>
+      <c r="K90" s="12"/>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>88</v>
+      </c>
+      <c r="B91" s="12"/>
+      <c r="C91" s="12"/>
+      <c r="D91" s="12"/>
+      <c r="E91" s="12"/>
+      <c r="F91" s="12"/>
+      <c r="G91" s="12"/>
+      <c r="H91" s="12"/>
+      <c r="I91" s="12"/>
+      <c r="J91" s="12"/>
+      <c r="K91" s="12"/>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>89</v>
+      </c>
+      <c r="B92" s="12"/>
+      <c r="C92" s="12"/>
+      <c r="D92" s="12"/>
+      <c r="E92" s="12"/>
+      <c r="F92" s="12"/>
+      <c r="G92" s="12"/>
+      <c r="H92" s="12"/>
+      <c r="I92" s="12"/>
+      <c r="J92" s="12"/>
+      <c r="K92" s="12"/>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>90</v>
+      </c>
+      <c r="B93" s="12"/>
+      <c r="C93" s="12"/>
+      <c r="D93" s="12"/>
+      <c r="E93" s="12"/>
+      <c r="F93" s="12"/>
+      <c r="G93" s="12"/>
+      <c r="H93" s="12"/>
+      <c r="I93" s="12"/>
+      <c r="J93" s="12"/>
+      <c r="K93" s="12"/>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>91</v>
+      </c>
+      <c r="B94" s="12"/>
+      <c r="C94" s="12"/>
+      <c r="D94" s="12"/>
+      <c r="E94" s="12"/>
+      <c r="F94" s="12"/>
+      <c r="G94" s="12"/>
+      <c r="H94" s="12"/>
+      <c r="I94" s="12"/>
+      <c r="J94" s="12"/>
+      <c r="K94" s="12"/>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>92</v>
+      </c>
+      <c r="B95" s="12"/>
+      <c r="C95" s="12"/>
+      <c r="D95" s="12"/>
+      <c r="E95" s="12"/>
+      <c r="F95" s="12"/>
+      <c r="G95" s="12"/>
+      <c r="H95" s="12"/>
+      <c r="I95" s="12"/>
+      <c r="J95" s="12"/>
+      <c r="K95" s="12"/>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>93</v>
+      </c>
+      <c r="B96" s="12"/>
+      <c r="C96" s="12"/>
+      <c r="D96" s="12"/>
+      <c r="E96" s="12"/>
+      <c r="F96" s="12"/>
+      <c r="G96" s="12"/>
+      <c r="H96" s="12"/>
+      <c r="I96" s="12"/>
+      <c r="J96" s="12"/>
+      <c r="K96" s="12"/>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>94</v>
+      </c>
+      <c r="B97" s="12"/>
+      <c r="C97" s="12"/>
+      <c r="D97" s="12"/>
+      <c r="E97" s="12"/>
+      <c r="F97" s="12"/>
+      <c r="G97" s="12"/>
+      <c r="H97" s="12"/>
+      <c r="I97" s="12"/>
+      <c r="J97" s="12"/>
+      <c r="K97" s="12"/>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>95</v>
+      </c>
+      <c r="B98" s="12"/>
+      <c r="C98" s="12"/>
+      <c r="D98" s="12"/>
+      <c r="E98" s="12"/>
+      <c r="F98" s="12"/>
+      <c r="G98" s="12"/>
+      <c r="H98" s="12"/>
+      <c r="I98" s="12"/>
+      <c r="J98" s="12"/>
+      <c r="K98" s="12"/>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>96</v>
+      </c>
+      <c r="B99" s="12"/>
+      <c r="C99" s="12"/>
+      <c r="D99" s="12"/>
+      <c r="E99" s="12"/>
+      <c r="F99" s="12"/>
+      <c r="G99" s="12"/>
+      <c r="H99" s="12"/>
+      <c r="I99" s="12"/>
+      <c r="J99" s="12"/>
+      <c r="K99" s="12"/>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>97</v>
+      </c>
+      <c r="B100" s="12"/>
+      <c r="C100" s="12"/>
+      <c r="D100" s="12"/>
+      <c r="E100" s="12"/>
+      <c r="F100" s="12"/>
+      <c r="G100" s="12"/>
+      <c r="H100" s="12"/>
+      <c r="I100" s="12"/>
+      <c r="J100" s="12"/>
+      <c r="K100" s="12"/>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>98</v>
+      </c>
+      <c r="B101" s="12"/>
+      <c r="C101" s="12"/>
+      <c r="D101" s="12"/>
+      <c r="E101" s="12"/>
+      <c r="F101" s="12"/>
+      <c r="G101" s="12"/>
+      <c r="H101" s="12"/>
+      <c r="I101" s="12"/>
+      <c r="J101" s="12"/>
+      <c r="K101" s="12"/>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>99</v>
+      </c>
+      <c r="B102" s="12"/>
+      <c r="C102" s="12"/>
+      <c r="D102" s="12"/>
+      <c r="E102" s="12"/>
+      <c r="F102" s="12"/>
+      <c r="G102" s="12"/>
+      <c r="H102" s="12"/>
+      <c r="I102" s="12"/>
+      <c r="J102" s="12"/>
+      <c r="K102" s="12"/>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>100</v>
+      </c>
+      <c r="B103" s="12"/>
+      <c r="C103" s="12"/>
+      <c r="D103" s="12"/>
+      <c r="E103" s="12"/>
+      <c r="F103" s="12"/>
+      <c r="G103" s="12"/>
+      <c r="H103" s="12"/>
+      <c r="I103" s="12"/>
+      <c r="J103" s="12"/>
+      <c r="K103" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,11 +3035,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed enemy attack rate and damage to values from spreadsheet
</commit_message>
<xml_diff>
--- a/Ressources/Documentation/RPG Stats Spreadsheet.xlsx
+++ b/Ressources/Documentation/RPG Stats Spreadsheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4B49CBA9-806A-4515-B430-45B37FCE48A1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{FB96D13C-A0CB-40F0-802E-8025BAD91ADF}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Soul" sheetId="3" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="59">
   <si>
     <t>Player Level</t>
   </si>
@@ -197,6 +197,21 @@
   <si>
     <t>XP to
 level up</t>
+  </si>
+  <si>
+    <t>Calculator DPS in WaitTime</t>
+  </si>
+  <si>
+    <t>DPS</t>
+  </si>
+  <si>
+    <t>Damage</t>
+  </si>
+  <si>
+    <t>WaitTime</t>
+  </si>
+  <si>
+    <t>HitSpeed</t>
   </si>
 </sst>
 </file>
@@ -897,7 +912,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1128,7 +1143,7 @@
         <v>280</v>
       </c>
       <c r="F6" s="12">
-        <f t="shared" ref="F6:G23" si="9">F5+$F$3</f>
+        <f t="shared" ref="F6:F23" si="9">F5+$F$3</f>
         <v>20</v>
       </c>
       <c r="G6" s="12">
@@ -3375,10 +3390,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEF27858-E5AD-4301-84CC-4CB96A95E69D}">
-  <dimension ref="A1:AG23"/>
+  <dimension ref="A1:AG30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AG3" sqref="AG3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3570,7 +3585,7 @@
         <v>2</v>
       </c>
       <c r="K3" s="24">
-        <v>1.5</v>
+        <v>1.8</v>
       </c>
       <c r="L3" s="24">
         <v>0.7</v>
@@ -3615,13 +3630,13 @@
         <v>1</v>
       </c>
       <c r="AD3" s="42">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AE3" s="42">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF3" s="42">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="AG3" s="42">
         <v>2</v>
@@ -3646,7 +3661,7 @@
         <v>10</v>
       </c>
       <c r="G4" s="12">
-        <f>F4/$G$3</f>
+        <f>F4*$G$3</f>
         <v>10</v>
       </c>
       <c r="H4" s="12">
@@ -3659,11 +3674,11 @@
       </c>
       <c r="K4" s="12">
         <f>$B4*K$3</f>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L4" s="12">
-        <f>K4/L$3</f>
-        <v>21.428571428571431</v>
+        <f>K4*L$3</f>
+        <v>12.6</v>
       </c>
       <c r="M4" s="12">
         <f>$C4*M$3</f>
@@ -3678,8 +3693,8 @@
         <v>5</v>
       </c>
       <c r="Q4" s="12">
-        <f>P4/Q$3</f>
-        <v>3.3333333333333335</v>
+        <f>P4*Q$3</f>
+        <v>7.5</v>
       </c>
       <c r="R4" s="12">
         <f>$C4*R$3</f>
@@ -3694,7 +3709,7 @@
         <v>4</v>
       </c>
       <c r="V4" s="12">
-        <f>U4/V$3</f>
+        <f>U4*V$3</f>
         <v>4</v>
       </c>
       <c r="W4" s="12">
@@ -3710,8 +3725,8 @@
         <v>15</v>
       </c>
       <c r="AA4" s="12">
-        <f>Z4/AA$3</f>
-        <v>30</v>
+        <f>Z4*AA$3</f>
+        <v>7.5</v>
       </c>
       <c r="AB4" s="12">
         <f>$C4*AB$3</f>
@@ -3719,15 +3734,15 @@
       </c>
       <c r="AD4" s="12">
         <f>$A4*AD$3</f>
-        <v>80</v>
+        <v>200</v>
       </c>
       <c r="AE4" s="12">
         <f>$B4*AE$3</f>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="AF4" s="12">
-        <f>AE4/AF$3</f>
-        <v>20</v>
+        <f>AE4*AF$3</f>
+        <v>24</v>
       </c>
       <c r="AG4" s="12">
         <f>$C4*AG$3</f>
@@ -3753,7 +3768,7 @@
         <v>12</v>
       </c>
       <c r="G5" s="12">
-        <f t="shared" ref="G5:G23" si="2">F5/$G$3</f>
+        <f t="shared" ref="G5:G23" si="2">F5*$G$3</f>
         <v>12</v>
       </c>
       <c r="H5" s="12">
@@ -3766,11 +3781,11 @@
       </c>
       <c r="K5" s="12">
         <f t="shared" ref="K5:K23" si="5">$B5*K$3</f>
-        <v>18</v>
+        <v>21.6</v>
       </c>
       <c r="L5" s="12">
-        <f t="shared" ref="L5:L23" si="6">K5/L$3</f>
-        <v>25.714285714285715</v>
+        <f t="shared" ref="L5:L23" si="6">K5*L$3</f>
+        <v>15.12</v>
       </c>
       <c r="M5" s="12">
         <f t="shared" ref="M5:M23" si="7">$C5*M$3</f>
@@ -3785,8 +3800,8 @@
         <v>6</v>
       </c>
       <c r="Q5" s="12">
-        <f t="shared" ref="Q5:Q23" si="10">P5/Q$3</f>
-        <v>4</v>
+        <f t="shared" ref="Q5:Q23" si="10">P5*Q$3</f>
+        <v>9</v>
       </c>
       <c r="R5" s="12">
         <f t="shared" ref="R5:R23" si="11">$C5*R$3</f>
@@ -3801,7 +3816,7 @@
         <v>4.8000000000000007</v>
       </c>
       <c r="V5" s="12">
-        <f t="shared" ref="V5:V23" si="14">U5/V$3</f>
+        <f t="shared" ref="V5:V23" si="14">U5*V$3</f>
         <v>4.8000000000000007</v>
       </c>
       <c r="W5" s="12">
@@ -3817,8 +3832,8 @@
         <v>18</v>
       </c>
       <c r="AA5" s="12">
-        <f t="shared" ref="AA5:AA23" si="18">Z5/AA$3</f>
-        <v>36</v>
+        <f t="shared" ref="AA5:AA23" si="18">Z5*AA$3</f>
+        <v>9</v>
       </c>
       <c r="AB5" s="12">
         <f t="shared" ref="AB5:AB23" si="19">$C5*AB$3</f>
@@ -3826,15 +3841,15 @@
       </c>
       <c r="AD5" s="12">
         <f t="shared" ref="AD5:AD23" si="20">$A5*AD$3</f>
-        <v>120</v>
+        <v>300</v>
       </c>
       <c r="AE5" s="12">
         <f t="shared" ref="AE5:AE23" si="21">$B5*AE$3</f>
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="AF5" s="12">
-        <f t="shared" ref="AF5:AF23" si="22">AE5/AF$3</f>
-        <v>24</v>
+        <f t="shared" ref="AF5:AF23" si="22">AE5*AF$3</f>
+        <v>28.8</v>
       </c>
       <c r="AG5" s="12">
         <f t="shared" ref="AG5:AG23" si="23">$C5*AG$3</f>
@@ -3873,11 +3888,11 @@
       </c>
       <c r="K6" s="12">
         <f t="shared" si="5"/>
-        <v>21</v>
+        <v>25.2</v>
       </c>
       <c r="L6" s="12">
         <f t="shared" si="6"/>
-        <v>30.000000000000004</v>
+        <v>17.639999999999997</v>
       </c>
       <c r="M6" s="12">
         <f t="shared" si="7"/>
@@ -3893,7 +3908,7 @@
       </c>
       <c r="Q6" s="12">
         <f t="shared" si="10"/>
-        <v>4.666666666666667</v>
+        <v>10.5</v>
       </c>
       <c r="R6" s="12">
         <f t="shared" si="11"/>
@@ -3925,7 +3940,7 @@
       </c>
       <c r="AA6" s="12">
         <f t="shared" si="18"/>
-        <v>42</v>
+        <v>10.5</v>
       </c>
       <c r="AB6" s="12">
         <f t="shared" si="19"/>
@@ -3933,15 +3948,15 @@
       </c>
       <c r="AD6" s="12">
         <f t="shared" si="20"/>
-        <v>160</v>
+        <v>400</v>
       </c>
       <c r="AE6" s="12">
         <f t="shared" si="21"/>
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="AF6" s="12">
         <f t="shared" si="22"/>
-        <v>28</v>
+        <v>33.6</v>
       </c>
       <c r="AG6" s="12">
         <f t="shared" si="23"/>
@@ -3980,11 +3995,11 @@
       </c>
       <c r="K7" s="12">
         <f t="shared" si="5"/>
-        <v>24</v>
+        <v>28.8</v>
       </c>
       <c r="L7" s="12">
         <f t="shared" si="6"/>
-        <v>34.285714285714285</v>
+        <v>20.16</v>
       </c>
       <c r="M7" s="12">
         <f t="shared" si="7"/>
@@ -4000,7 +4015,7 @@
       </c>
       <c r="Q7" s="12">
         <f t="shared" si="10"/>
-        <v>5.333333333333333</v>
+        <v>12</v>
       </c>
       <c r="R7" s="12">
         <f t="shared" si="11"/>
@@ -4032,7 +4047,7 @@
       </c>
       <c r="AA7" s="12">
         <f t="shared" si="18"/>
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="AB7" s="12">
         <f t="shared" si="19"/>
@@ -4040,15 +4055,15 @@
       </c>
       <c r="AD7" s="12">
         <f t="shared" si="20"/>
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="AE7" s="12">
         <f t="shared" si="21"/>
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="AF7" s="12">
         <f t="shared" si="22"/>
-        <v>32</v>
+        <v>38.400000000000006</v>
       </c>
       <c r="AG7" s="12">
         <f t="shared" si="23"/>
@@ -4087,11 +4102,11 @@
       </c>
       <c r="K8" s="12">
         <f t="shared" si="5"/>
-        <v>27</v>
+        <v>32.4</v>
       </c>
       <c r="L8" s="12">
         <f t="shared" si="6"/>
-        <v>38.571428571428577</v>
+        <v>22.679999999999996</v>
       </c>
       <c r="M8" s="12">
         <f t="shared" si="7"/>
@@ -4107,7 +4122,7 @@
       </c>
       <c r="Q8" s="12">
         <f t="shared" si="10"/>
-        <v>6</v>
+        <v>13.5</v>
       </c>
       <c r="R8" s="12">
         <f t="shared" si="11"/>
@@ -4139,7 +4154,7 @@
       </c>
       <c r="AA8" s="12">
         <f t="shared" si="18"/>
-        <v>54</v>
+        <v>13.5</v>
       </c>
       <c r="AB8" s="12">
         <f t="shared" si="19"/>
@@ -4147,15 +4162,15 @@
       </c>
       <c r="AD8" s="12">
         <f t="shared" si="20"/>
-        <v>240</v>
+        <v>600</v>
       </c>
       <c r="AE8" s="12">
         <f t="shared" si="21"/>
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="AF8" s="12">
         <f t="shared" si="22"/>
-        <v>36</v>
+        <v>43.2</v>
       </c>
       <c r="AG8" s="12">
         <f t="shared" si="23"/>
@@ -4194,11 +4209,11 @@
       </c>
       <c r="K9" s="12">
         <f t="shared" si="5"/>
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="L9" s="12">
         <f t="shared" si="6"/>
-        <v>42.857142857142861</v>
+        <v>25.2</v>
       </c>
       <c r="M9" s="12">
         <f t="shared" si="7"/>
@@ -4214,7 +4229,7 @@
       </c>
       <c r="Q9" s="12">
         <f t="shared" si="10"/>
-        <v>6.666666666666667</v>
+        <v>15</v>
       </c>
       <c r="R9" s="12">
         <f t="shared" si="11"/>
@@ -4246,7 +4261,7 @@
       </c>
       <c r="AA9" s="12">
         <f t="shared" si="18"/>
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="AB9" s="12">
         <f t="shared" si="19"/>
@@ -4254,15 +4269,15 @@
       </c>
       <c r="AD9" s="12">
         <f t="shared" si="20"/>
-        <v>280</v>
+        <v>700</v>
       </c>
       <c r="AE9" s="12">
         <f t="shared" si="21"/>
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="AF9" s="12">
         <f t="shared" si="22"/>
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="AG9" s="12">
         <f t="shared" si="23"/>
@@ -4301,11 +4316,11 @@
       </c>
       <c r="K10" s="12">
         <f t="shared" si="5"/>
-        <v>33</v>
+        <v>39.6</v>
       </c>
       <c r="L10" s="12">
         <f t="shared" si="6"/>
-        <v>47.142857142857146</v>
+        <v>27.72</v>
       </c>
       <c r="M10" s="12">
         <f t="shared" si="7"/>
@@ -4321,7 +4336,7 @@
       </c>
       <c r="Q10" s="12">
         <f t="shared" si="10"/>
-        <v>7.333333333333333</v>
+        <v>16.5</v>
       </c>
       <c r="R10" s="12">
         <f t="shared" si="11"/>
@@ -4353,7 +4368,7 @@
       </c>
       <c r="AA10" s="12">
         <f t="shared" si="18"/>
-        <v>66</v>
+        <v>16.5</v>
       </c>
       <c r="AB10" s="12">
         <f t="shared" si="19"/>
@@ -4361,15 +4376,15 @@
       </c>
       <c r="AD10" s="12">
         <f t="shared" si="20"/>
-        <v>320</v>
+        <v>800</v>
       </c>
       <c r="AE10" s="12">
         <f t="shared" si="21"/>
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="AF10" s="12">
         <f t="shared" si="22"/>
-        <v>44</v>
+        <v>52.800000000000004</v>
       </c>
       <c r="AG10" s="12">
         <f t="shared" si="23"/>
@@ -4408,11 +4423,11 @@
       </c>
       <c r="K11" s="12">
         <f t="shared" si="5"/>
-        <v>36</v>
+        <v>43.2</v>
       </c>
       <c r="L11" s="12">
         <f t="shared" si="6"/>
-        <v>51.428571428571431</v>
+        <v>30.24</v>
       </c>
       <c r="M11" s="12">
         <f t="shared" si="7"/>
@@ -4428,7 +4443,7 @@
       </c>
       <c r="Q11" s="12">
         <f t="shared" si="10"/>
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="R11" s="12">
         <f t="shared" si="11"/>
@@ -4460,7 +4475,7 @@
       </c>
       <c r="AA11" s="12">
         <f t="shared" si="18"/>
-        <v>72</v>
+        <v>18</v>
       </c>
       <c r="AB11" s="12">
         <f t="shared" si="19"/>
@@ -4468,15 +4483,15 @@
       </c>
       <c r="AD11" s="12">
         <f t="shared" si="20"/>
-        <v>360</v>
+        <v>900</v>
       </c>
       <c r="AE11" s="12">
         <f t="shared" si="21"/>
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="AF11" s="12">
         <f t="shared" si="22"/>
-        <v>48</v>
+        <v>57.6</v>
       </c>
       <c r="AG11" s="12">
         <f t="shared" si="23"/>
@@ -4515,11 +4530,11 @@
       </c>
       <c r="K12" s="12">
         <f t="shared" si="5"/>
-        <v>39</v>
+        <v>46.800000000000004</v>
       </c>
       <c r="L12" s="12">
         <f t="shared" si="6"/>
-        <v>55.714285714285715</v>
+        <v>32.76</v>
       </c>
       <c r="M12" s="12">
         <f t="shared" si="7"/>
@@ -4535,7 +4550,7 @@
       </c>
       <c r="Q12" s="12">
         <f t="shared" si="10"/>
-        <v>8.6666666666666661</v>
+        <v>19.5</v>
       </c>
       <c r="R12" s="12">
         <f t="shared" si="11"/>
@@ -4567,7 +4582,7 @@
       </c>
       <c r="AA12" s="12">
         <f t="shared" si="18"/>
-        <v>78</v>
+        <v>19.5</v>
       </c>
       <c r="AB12" s="12">
         <f t="shared" si="19"/>
@@ -4575,15 +4590,15 @@
       </c>
       <c r="AD12" s="12">
         <f t="shared" si="20"/>
-        <v>400</v>
+        <v>1000</v>
       </c>
       <c r="AE12" s="12">
         <f t="shared" si="21"/>
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="AF12" s="12">
         <f t="shared" si="22"/>
-        <v>52</v>
+        <v>62.400000000000006</v>
       </c>
       <c r="AG12" s="12">
         <f t="shared" si="23"/>
@@ -4622,11 +4637,11 @@
       </c>
       <c r="K13" s="12">
         <f t="shared" si="5"/>
-        <v>42</v>
+        <v>50.4</v>
       </c>
       <c r="L13" s="12">
         <f t="shared" si="6"/>
-        <v>60.000000000000007</v>
+        <v>35.279999999999994</v>
       </c>
       <c r="M13" s="12">
         <f t="shared" si="7"/>
@@ -4642,7 +4657,7 @@
       </c>
       <c r="Q13" s="12">
         <f t="shared" si="10"/>
-        <v>9.3333333333333339</v>
+        <v>21</v>
       </c>
       <c r="R13" s="12">
         <f t="shared" si="11"/>
@@ -4674,7 +4689,7 @@
       </c>
       <c r="AA13" s="12">
         <f t="shared" si="18"/>
-        <v>84</v>
+        <v>21</v>
       </c>
       <c r="AB13" s="12">
         <f t="shared" si="19"/>
@@ -4682,15 +4697,15 @@
       </c>
       <c r="AD13" s="12">
         <f t="shared" si="20"/>
-        <v>440</v>
+        <v>1100</v>
       </c>
       <c r="AE13" s="12">
         <f t="shared" si="21"/>
-        <v>56</v>
+        <v>84</v>
       </c>
       <c r="AF13" s="12">
         <f t="shared" si="22"/>
-        <v>56</v>
+        <v>67.2</v>
       </c>
       <c r="AG13" s="12">
         <f t="shared" si="23"/>
@@ -4729,11 +4744,11 @@
       </c>
       <c r="K14" s="12">
         <f t="shared" si="5"/>
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="L14" s="12">
         <f t="shared" si="6"/>
-        <v>64.285714285714292</v>
+        <v>37.799999999999997</v>
       </c>
       <c r="M14" s="12">
         <f t="shared" si="7"/>
@@ -4749,7 +4764,7 @@
       </c>
       <c r="Q14" s="12">
         <f t="shared" si="10"/>
-        <v>10</v>
+        <v>22.5</v>
       </c>
       <c r="R14" s="12">
         <f t="shared" si="11"/>
@@ -4781,7 +4796,7 @@
       </c>
       <c r="AA14" s="12">
         <f t="shared" si="18"/>
-        <v>90</v>
+        <v>22.5</v>
       </c>
       <c r="AB14" s="12">
         <f t="shared" si="19"/>
@@ -4789,15 +4804,15 @@
       </c>
       <c r="AD14" s="12">
         <f t="shared" si="20"/>
-        <v>480</v>
+        <v>1200</v>
       </c>
       <c r="AE14" s="12">
         <f t="shared" si="21"/>
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="AF14" s="12">
         <f t="shared" si="22"/>
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="AG14" s="12">
         <f t="shared" si="23"/>
@@ -4836,11 +4851,11 @@
       </c>
       <c r="K15" s="12">
         <f t="shared" si="5"/>
-        <v>48</v>
+        <v>57.6</v>
       </c>
       <c r="L15" s="12">
         <f t="shared" si="6"/>
-        <v>68.571428571428569</v>
+        <v>40.32</v>
       </c>
       <c r="M15" s="12">
         <f t="shared" si="7"/>
@@ -4856,7 +4871,7 @@
       </c>
       <c r="Q15" s="12">
         <f t="shared" si="10"/>
-        <v>10.666666666666666</v>
+        <v>24</v>
       </c>
       <c r="R15" s="12">
         <f t="shared" si="11"/>
@@ -4888,7 +4903,7 @@
       </c>
       <c r="AA15" s="12">
         <f t="shared" si="18"/>
-        <v>96</v>
+        <v>24</v>
       </c>
       <c r="AB15" s="12">
         <f t="shared" si="19"/>
@@ -4896,15 +4911,15 @@
       </c>
       <c r="AD15" s="12">
         <f t="shared" si="20"/>
-        <v>520</v>
+        <v>1300</v>
       </c>
       <c r="AE15" s="12">
         <f t="shared" si="21"/>
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="AF15" s="12">
         <f t="shared" si="22"/>
-        <v>64</v>
+        <v>76.800000000000011</v>
       </c>
       <c r="AG15" s="12">
         <f t="shared" si="23"/>
@@ -4943,11 +4958,11 @@
       </c>
       <c r="K16" s="12">
         <f t="shared" si="5"/>
-        <v>51</v>
+        <v>61.2</v>
       </c>
       <c r="L16" s="12">
         <f t="shared" si="6"/>
-        <v>72.857142857142861</v>
+        <v>42.839999999999996</v>
       </c>
       <c r="M16" s="12">
         <f t="shared" si="7"/>
@@ -4963,7 +4978,7 @@
       </c>
       <c r="Q16" s="12">
         <f t="shared" si="10"/>
-        <v>11.333333333333334</v>
+        <v>25.5</v>
       </c>
       <c r="R16" s="12">
         <f t="shared" si="11"/>
@@ -4995,7 +5010,7 @@
       </c>
       <c r="AA16" s="12">
         <f t="shared" si="18"/>
-        <v>102</v>
+        <v>25.5</v>
       </c>
       <c r="AB16" s="12">
         <f t="shared" si="19"/>
@@ -5003,15 +5018,15 @@
       </c>
       <c r="AD16" s="12">
         <f t="shared" si="20"/>
-        <v>560</v>
+        <v>1400</v>
       </c>
       <c r="AE16" s="12">
         <f t="shared" si="21"/>
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="AF16" s="12">
         <f t="shared" si="22"/>
-        <v>68</v>
+        <v>81.600000000000009</v>
       </c>
       <c r="AG16" s="12">
         <f t="shared" si="23"/>
@@ -5050,11 +5065,11 @@
       </c>
       <c r="K17" s="12">
         <f t="shared" si="5"/>
-        <v>54</v>
+        <v>64.8</v>
       </c>
       <c r="L17" s="12">
         <f t="shared" si="6"/>
-        <v>77.142857142857153</v>
+        <v>45.359999999999992</v>
       </c>
       <c r="M17" s="12">
         <f t="shared" si="7"/>
@@ -5070,7 +5085,7 @@
       </c>
       <c r="Q17" s="12">
         <f t="shared" si="10"/>
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="R17" s="12">
         <f t="shared" si="11"/>
@@ -5102,7 +5117,7 @@
       </c>
       <c r="AA17" s="12">
         <f t="shared" si="18"/>
-        <v>108</v>
+        <v>27</v>
       </c>
       <c r="AB17" s="12">
         <f t="shared" si="19"/>
@@ -5110,15 +5125,15 @@
       </c>
       <c r="AD17" s="12">
         <f t="shared" si="20"/>
-        <v>600</v>
+        <v>1500</v>
       </c>
       <c r="AE17" s="12">
         <f t="shared" si="21"/>
-        <v>72</v>
+        <v>108</v>
       </c>
       <c r="AF17" s="12">
         <f t="shared" si="22"/>
-        <v>72</v>
+        <v>86.4</v>
       </c>
       <c r="AG17" s="12">
         <f t="shared" si="23"/>
@@ -5157,11 +5172,11 @@
       </c>
       <c r="K18" s="12">
         <f t="shared" si="5"/>
-        <v>57</v>
+        <v>68.400000000000006</v>
       </c>
       <c r="L18" s="12">
         <f t="shared" si="6"/>
-        <v>81.428571428571431</v>
+        <v>47.88</v>
       </c>
       <c r="M18" s="12">
         <f t="shared" si="7"/>
@@ -5177,7 +5192,7 @@
       </c>
       <c r="Q18" s="12">
         <f t="shared" si="10"/>
-        <v>12.666666666666666</v>
+        <v>28.5</v>
       </c>
       <c r="R18" s="12">
         <f t="shared" si="11"/>
@@ -5209,7 +5224,7 @@
       </c>
       <c r="AA18" s="12">
         <f t="shared" si="18"/>
-        <v>114</v>
+        <v>28.5</v>
       </c>
       <c r="AB18" s="12">
         <f t="shared" si="19"/>
@@ -5217,15 +5232,15 @@
       </c>
       <c r="AD18" s="12">
         <f t="shared" si="20"/>
-        <v>640</v>
+        <v>1600</v>
       </c>
       <c r="AE18" s="12">
         <f t="shared" si="21"/>
-        <v>76</v>
+        <v>114</v>
       </c>
       <c r="AF18" s="12">
         <f t="shared" si="22"/>
-        <v>76</v>
+        <v>91.2</v>
       </c>
       <c r="AG18" s="12">
         <f t="shared" si="23"/>
@@ -5264,11 +5279,11 @@
       </c>
       <c r="K19" s="12">
         <f t="shared" si="5"/>
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="L19" s="12">
         <f t="shared" si="6"/>
-        <v>85.714285714285722</v>
+        <v>50.4</v>
       </c>
       <c r="M19" s="12">
         <f t="shared" si="7"/>
@@ -5284,7 +5299,7 @@
       </c>
       <c r="Q19" s="12">
         <f t="shared" si="10"/>
-        <v>13.333333333333334</v>
+        <v>30</v>
       </c>
       <c r="R19" s="12">
         <f t="shared" si="11"/>
@@ -5316,7 +5331,7 @@
       </c>
       <c r="AA19" s="12">
         <f t="shared" si="18"/>
-        <v>120</v>
+        <v>30</v>
       </c>
       <c r="AB19" s="12">
         <f t="shared" si="19"/>
@@ -5324,15 +5339,15 @@
       </c>
       <c r="AD19" s="12">
         <f t="shared" si="20"/>
-        <v>680</v>
+        <v>1700</v>
       </c>
       <c r="AE19" s="12">
         <f t="shared" si="21"/>
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="AF19" s="12">
         <f t="shared" si="22"/>
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="AG19" s="12">
         <f t="shared" si="23"/>
@@ -5371,11 +5386,11 @@
       </c>
       <c r="K20" s="12">
         <f t="shared" si="5"/>
-        <v>63</v>
+        <v>75.600000000000009</v>
       </c>
       <c r="L20" s="12">
         <f t="shared" si="6"/>
-        <v>90</v>
+        <v>52.92</v>
       </c>
       <c r="M20" s="12">
         <f t="shared" si="7"/>
@@ -5391,7 +5406,7 @@
       </c>
       <c r="Q20" s="12">
         <f t="shared" si="10"/>
-        <v>14</v>
+        <v>31.5</v>
       </c>
       <c r="R20" s="12">
         <f t="shared" si="11"/>
@@ -5423,7 +5438,7 @@
       </c>
       <c r="AA20" s="12">
         <f t="shared" si="18"/>
-        <v>126</v>
+        <v>31.5</v>
       </c>
       <c r="AB20" s="12">
         <f t="shared" si="19"/>
@@ -5431,15 +5446,15 @@
       </c>
       <c r="AD20" s="12">
         <f t="shared" si="20"/>
-        <v>720</v>
+        <v>1800</v>
       </c>
       <c r="AE20" s="12">
         <f t="shared" si="21"/>
-        <v>84</v>
+        <v>126</v>
       </c>
       <c r="AF20" s="12">
         <f t="shared" si="22"/>
-        <v>84</v>
+        <v>100.80000000000001</v>
       </c>
       <c r="AG20" s="12">
         <f t="shared" si="23"/>
@@ -5478,11 +5493,11 @@
       </c>
       <c r="K21" s="12">
         <f t="shared" si="5"/>
-        <v>66</v>
+        <v>79.2</v>
       </c>
       <c r="L21" s="12">
         <f t="shared" si="6"/>
-        <v>94.285714285714292</v>
+        <v>55.44</v>
       </c>
       <c r="M21" s="12">
         <f t="shared" si="7"/>
@@ -5498,7 +5513,7 @@
       </c>
       <c r="Q21" s="12">
         <f t="shared" si="10"/>
-        <v>14.666666666666666</v>
+        <v>33</v>
       </c>
       <c r="R21" s="12">
         <f t="shared" si="11"/>
@@ -5530,7 +5545,7 @@
       </c>
       <c r="AA21" s="12">
         <f t="shared" si="18"/>
-        <v>132</v>
+        <v>33</v>
       </c>
       <c r="AB21" s="12">
         <f t="shared" si="19"/>
@@ -5538,15 +5553,15 @@
       </c>
       <c r="AD21" s="12">
         <f t="shared" si="20"/>
-        <v>760</v>
+        <v>1900</v>
       </c>
       <c r="AE21" s="12">
         <f t="shared" si="21"/>
-        <v>88</v>
+        <v>132</v>
       </c>
       <c r="AF21" s="12">
         <f t="shared" si="22"/>
-        <v>88</v>
+        <v>105.60000000000001</v>
       </c>
       <c r="AG21" s="12">
         <f t="shared" si="23"/>
@@ -5585,11 +5600,11 @@
       </c>
       <c r="K22" s="12">
         <f t="shared" si="5"/>
-        <v>69</v>
+        <v>82.8</v>
       </c>
       <c r="L22" s="12">
         <f t="shared" si="6"/>
-        <v>98.571428571428584</v>
+        <v>57.959999999999994</v>
       </c>
       <c r="M22" s="12">
         <f t="shared" si="7"/>
@@ -5605,7 +5620,7 @@
       </c>
       <c r="Q22" s="12">
         <f t="shared" si="10"/>
-        <v>15.333333333333334</v>
+        <v>34.5</v>
       </c>
       <c r="R22" s="12">
         <f t="shared" si="11"/>
@@ -5637,7 +5652,7 @@
       </c>
       <c r="AA22" s="12">
         <f t="shared" si="18"/>
-        <v>138</v>
+        <v>34.5</v>
       </c>
       <c r="AB22" s="12">
         <f t="shared" si="19"/>
@@ -5645,15 +5660,15 @@
       </c>
       <c r="AD22" s="12">
         <f t="shared" si="20"/>
-        <v>800</v>
+        <v>2000</v>
       </c>
       <c r="AE22" s="12">
         <f t="shared" si="21"/>
-        <v>92</v>
+        <v>138</v>
       </c>
       <c r="AF22" s="12">
         <f t="shared" si="22"/>
-        <v>92</v>
+        <v>110.4</v>
       </c>
       <c r="AG22" s="12">
         <f t="shared" si="23"/>
@@ -5692,11 +5707,11 @@
       </c>
       <c r="K23" s="12">
         <f t="shared" si="5"/>
-        <v>72</v>
+        <v>86.4</v>
       </c>
       <c r="L23" s="12">
         <f t="shared" si="6"/>
-        <v>102.85714285714286</v>
+        <v>60.48</v>
       </c>
       <c r="M23" s="12">
         <f t="shared" si="7"/>
@@ -5712,7 +5727,7 @@
       </c>
       <c r="Q23" s="12">
         <f t="shared" si="10"/>
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="R23" s="12">
         <f t="shared" si="11"/>
@@ -5744,7 +5759,7 @@
       </c>
       <c r="AA23" s="12">
         <f t="shared" si="18"/>
-        <v>144</v>
+        <v>36</v>
       </c>
       <c r="AB23" s="12">
         <f t="shared" si="19"/>
@@ -5752,19 +5767,58 @@
       </c>
       <c r="AD23" s="12">
         <f t="shared" si="20"/>
-        <v>840</v>
+        <v>2100</v>
       </c>
       <c r="AE23" s="12">
         <f t="shared" si="21"/>
-        <v>96</v>
+        <v>144</v>
       </c>
       <c r="AF23" s="12">
         <f t="shared" si="22"/>
-        <v>96</v>
+        <v>115.2</v>
       </c>
       <c r="AG23" s="12">
         <f t="shared" si="23"/>
         <v>288</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29">
+        <f>B28*B27</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30">
+        <f>B28/B29</f>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>